<commit_message>
Update Analyse des resultatsV2.xlsx
</commit_message>
<xml_diff>
--- a/Project/Resultat/Analyse des resultatsV2.xlsx
+++ b/Project/Resultat/Analyse des resultatsV2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/464c61f4079a7534/Documents/GitHub/RecSys/Project/Resultat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{05055A83-D3E0-4BD4-8F83-76897CDF407D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{9E0C6F4F-3F99-45CC-8ADB-3051EA303054}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{05055A83-D3E0-4BD4-8F83-76897CDF407D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{A638E076-15CF-493E-A8E1-7A0547A61EF0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6648" xr2:uid="{D030182A-CDE3-42A1-BF6B-B30E0474A4FF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6648" activeTab="2" xr2:uid="{D030182A-CDE3-42A1-BF6B-B30E0474A4FF}"/>
   </bookViews>
   <sheets>
     <sheet name="MTH1006" sheetId="3" r:id="rId1"/>
@@ -6231,10 +6231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6075CE3-C5DE-4132-B6B7-199C55931189}">
-  <dimension ref="A2:N9"/>
+  <dimension ref="A2:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6312,6 +6312,24 @@
       <c r="F5" t="s">
         <v>134</v>
       </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
       <c r="N5">
         <v>1</v>
       </c>
@@ -6335,6 +6353,24 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
       <c r="N6">
         <v>2</v>
       </c>
@@ -6358,6 +6394,24 @@
       <c r="F7" t="s">
         <v>9</v>
       </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
       <c r="N7">
         <v>3</v>
       </c>
@@ -6381,6 +6435,24 @@
       <c r="F8" t="s">
         <v>22</v>
       </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
       <c r="N8">
         <v>4</v>
       </c>
@@ -6404,8 +6476,46 @@
       <c r="F9" t="s">
         <v>62</v>
       </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
       <c r="N9">
         <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.4</v>
+      </c>
+      <c r="B11">
+        <v>0.8</v>
+      </c>
+      <c r="C11">
+        <v>0.4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.2</v>
+      </c>
+      <c r="F11">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -6815,10 +6925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CD6A43-0763-4EC0-BB42-E304A873C144}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F9"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6904,6 +7014,24 @@
       <c r="F5" t="s">
         <v>43</v>
       </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
       <c r="N5">
         <v>1</v>
       </c>
@@ -6927,6 +7055,24 @@
       <c r="F6" t="s">
         <v>150</v>
       </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
       <c r="N6">
         <v>2</v>
       </c>
@@ -6950,6 +7096,24 @@
       <c r="F7" t="s">
         <v>114</v>
       </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
       <c r="N7">
         <v>3</v>
       </c>
@@ -6973,6 +7137,24 @@
       <c r="F8" t="s">
         <v>158</v>
       </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
       <c r="N8">
         <v>4</v>
       </c>
@@ -6996,8 +7178,46 @@
       <c r="F9" t="s">
         <v>156</v>
       </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
       <c r="N9">
         <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0.2</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -7017,8 +7237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67507C4B-FE4A-4529-9CE9-3A2B1154733A}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7104,6 +7324,24 @@
       <c r="F5" t="s">
         <v>159</v>
       </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
       <c r="N5">
         <v>1</v>
       </c>
@@ -7127,6 +7365,24 @@
       <c r="F6" t="s">
         <v>165</v>
       </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
       <c r="N6">
         <v>2</v>
       </c>
@@ -7150,6 +7406,24 @@
       <c r="F7" t="s">
         <v>168</v>
       </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
       <c r="N7">
         <v>3</v>
       </c>
@@ -7173,6 +7447,24 @@
       <c r="F8" t="s">
         <v>161</v>
       </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
       <c r="N8">
         <v>4</v>
       </c>
@@ -7195,6 +7487,24 @@
       </c>
       <c r="F9" t="s">
         <v>172</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
       </c>
       <c r="N9">
         <v>5</v>

</xml_diff>